<commit_message>
more updates to poltava
</commit_message>
<xml_diff>
--- a/t2dm-poltava/t2dm_poltava_databook.xlsx
+++ b/t2dm-poltava/t2dm_poltava_databook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/cascade-analyses/t2dm-poltava/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB32A927-EFDB-1F46-8482-147646DF2761}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277EC250-887E-4940-B6F3-AC8C21124BDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="19260" windowHeight="16180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="19260" windowHeight="16180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -23124,8 +23124,8 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23846,8 +23846,8 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23994,7 +23994,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="4">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -24349,7 +24349,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="4">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>8</v>
@@ -24395,7 +24395,7 @@
         <v>24</v>
       </c>
       <c r="C32" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>8</v>
@@ -24515,7 +24515,7 @@
       <formula>AND(COUNTIF(E35:H35,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B5 B20 B17 B11 B2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
@@ -24536,7 +24536,7 @@
   <dimension ref="B3:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:H29"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>